<commit_message>
new version of puzzle 2
</commit_message>
<xml_diff>
--- a/trojanHorse.xlsx
+++ b/trojanHorse.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
   <si>
     <t>MAN</t>
   </si>
@@ -69,15 +69,6 @@
     <t>?CITY</t>
   </si>
   <si>
-    <t>?HORSE</t>
-  </si>
-  <si>
-    <t>GOOD</t>
-  </si>
-  <si>
-    <t>ANIMAL</t>
-  </si>
-  <si>
     <t>MONEY</t>
   </si>
   <si>
@@ -141,9 +132,6 @@
     <t>?SHIP</t>
   </si>
   <si>
-    <t>?FAR</t>
-  </si>
-  <si>
     <t>?TRAVEL</t>
   </si>
   <si>
@@ -156,19 +144,31 @@
     <t>?EXIT</t>
   </si>
   <si>
-    <t>?DOOR</t>
-  </si>
-  <si>
-    <t>?OPEN</t>
-  </si>
-  <si>
     <t>?WIN</t>
   </si>
   <si>
-    <t>?MANY</t>
-  </si>
-  <si>
     <t xml:space="preserve">Find in Puzzle 3 </t>
+  </si>
+  <si>
+    <t>TRAVEL</t>
+  </si>
+  <si>
+    <t>SHIP</t>
+  </si>
+  <si>
+    <t>FAR</t>
+  </si>
+  <si>
+    <t>EXIT</t>
+  </si>
+  <si>
+    <t>Known From Puzzle 2</t>
+  </si>
+  <si>
+    <t>KING</t>
+  </si>
+  <si>
+    <t>FOR</t>
   </si>
 </sst>
 </file>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,37 +509,43 @@
     <col min="16" max="16" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
       <c r="L2" t="s">
         <v>2</v>
@@ -547,33 +553,39 @@
       <c r="N2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="L3" t="s">
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="P3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N4" t="s">
         <v>1</v>
@@ -581,22 +593,25 @@
       <c r="P4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
         <v>2</v>
@@ -604,50 +619,62 @@
       <c r="P5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="R7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="R8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,152 +682,264 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="L9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" t="s">
+        <v>27</v>
+      </c>
+      <c r="R9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="N9" t="s">
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="R12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="N11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
       <c r="N14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
       <c r="N16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
       <c r="N17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I19" t="s">
-        <v>47</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="I28" t="s">
+        <v>41</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implement puzzle 3 add connected words
</commit_message>
<xml_diff>
--- a/trojanHorse.xlsx
+++ b/trojanHorse.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="27465" windowHeight="7245"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="24000" windowHeight="7245"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="51">
   <si>
     <t>MAN</t>
   </si>
@@ -42,12 +42,6 @@
     <t>HORSE</t>
   </si>
   <si>
-    <t>OPEN</t>
-  </si>
-  <si>
-    <t>DOOR</t>
-  </si>
-  <si>
     <t>STEAL</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>SHIP</t>
   </si>
   <si>
-    <t>FAR</t>
-  </si>
-  <si>
     <t>EXIT</t>
   </si>
   <si>
@@ -169,6 +160,18 @@
   </si>
   <si>
     <t>FOR</t>
+  </si>
+  <si>
+    <t>QUEEN</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>woman</t>
+  </si>
+  <si>
+    <t>FIND</t>
   </si>
 </sst>
 </file>
@@ -488,7 +491,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -499,7 +502,7 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,32 +520,32 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="L1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -562,116 +565,110 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="R3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N4" t="s">
         <v>1</v>
       </c>
-      <c r="P4" t="s">
-        <v>8</v>
-      </c>
       <c r="R4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N5" t="s">
         <v>2</v>
       </c>
       <c r="P5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="R6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>50</v>
+      </c>
       <c r="N8" t="s">
-        <v>26</v>
-      </c>
-      <c r="R8" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -682,67 +679,67 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N9" t="s">
-        <v>27</v>
-      </c>
-      <c r="R9" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="N10" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="L11" t="s">
+        <v>48</v>
       </c>
       <c r="N11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="R11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>49</v>
+      </c>
       <c r="N12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -750,16 +747,16 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -767,23 +764,23 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>0</v>
@@ -792,38 +789,38 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="N16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
         <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>4</v>
@@ -835,41 +832,41 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -877,16 +874,16 @@
         <v>0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -894,10 +891,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -905,7 +902,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -916,7 +913,7 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>5</v>
@@ -925,22 +922,22 @@
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="I28" t="s">
-        <v>41</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>